<commit_message>
added pipeline to make a database that works with the website
</commit_message>
<xml_diff>
--- a/inputs/private_inputs/old_grassius_names.xlsx
+++ b/inputs/private_inputs/old_grassius_names.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">GRMZM2G152415</t>
   </si>
   <si>
-    <t xml:space="preserve">AP2-EREBP</t>
+    <t xml:space="preserve">AP2/ERF-ERF</t>
   </si>
   <si>
     <t xml:space="preserve">ZmEREB31</t>
@@ -26092,6 +26092,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -26176,7 +26177,7 @@
   <dimension ref="A1:E3010"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>